<commit_message>
Bug in code gefixed.
Definitieve versie van product backlog en user stories.
</commit_message>
<xml_diff>
--- a/Product_backlog_examen_programmingadvance_euromoon_Lilian_Levano.xlsx
+++ b/Product_backlog_examen_programmingadvance_euromoon_Lilian_Levano.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ehb-my.sharepoint.com/personal/lilian_levano_student_ehb_be/Documents/école ehb/cours/programming advanced prg1 s1/ExamenProjectEuromoon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="122" documentId="8_{C82A30B9-B475-4E18-AA91-DAFEC04BE60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{418F895F-A373-4D79-9D7D-EEC53FE98A6C}"/>
+  <xr:revisionPtr revIDLastSave="123" documentId="8_{C82A30B9-B475-4E18-AA91-DAFEC04BE60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6C1417F-B508-4904-A6F1-02261B559DAB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{F36CC0DA-C0BC-4E8B-805B-81862F0CC485}"/>
   </bookViews>
@@ -231,6 +231,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -643,7 +647,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="2:10" ht="294.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" ht="211.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Laatste commit and push
</commit_message>
<xml_diff>
--- a/Product_backlog_examen_programmingadvance_euromoon_Lilian_Levano.xlsx
+++ b/Product_backlog_examen_programmingadvance_euromoon_Lilian_Levano.xlsx
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7EF842B-8361-468E-9ADC-5E5571BF7441}">
   <dimension ref="B3:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>